<commit_message>
feat(dispa-link): dispa-link common mapping functions
</commit_message>
<xml_diff>
--- a/ConfigFiles/Config_EnergyScope.xlsx
+++ b/ConfigFiles/Config_EnergyScope.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\DispaSET-SideTools\ConfigFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Github\Dispa-LINK\ConfigFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7496D1-4819-4F19-B8F7-A1D5FB89A60F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4954E6E-DB49-41FB-88C2-212D658BD063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="244">
   <si>
     <t>Default value</t>
   </si>
@@ -756,6 +756,18 @@
   </si>
   <si>
     <t>Simulations/simulation_37500_ElecImport=0</t>
+  </si>
+  <si>
+    <t>CPLEX Accuracy</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>CPLEX Setting</t>
+  </si>
+  <si>
+    <t>Agressive</t>
   </si>
 </sst>
 </file>
@@ -916,7 +928,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1035,6 +1047,9 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1484,10 +1499,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H330"/>
+  <dimension ref="A1:J330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A274" workbookViewId="0">
+      <selection activeCell="E208" sqref="E208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1504,16 +1519,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
     </row>
     <row r="2" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1528,15 +1543,15 @@
     <row r="3" spans="1:8" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:8" s="31" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="30"/>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
@@ -1552,15 +1567,15 @@
       <c r="A6" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>209</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
     </row>
     <row r="7" spans="1:8" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="12"/>
@@ -1678,7 +1693,7 @@
     <row r="30" spans="1:2" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:2" ht="13.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:2" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:8" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="35" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
         <v>167</v>
       </c>
@@ -1690,7 +1705,7 @@
       <c r="G33" s="33"/>
       <c r="H33" s="33"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>34</v>
       </c>
@@ -1705,7 +1720,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
@@ -1719,7 +1734,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
@@ -1733,7 +1748,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>84</v>
       </c>
@@ -1742,7 +1757,7 @@
       </c>
       <c r="C37" s="4"/>
     </row>
-    <row r="38" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>128</v>
       </c>
@@ -1754,16 +1769,36 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="C39" s="41">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="I40" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:10" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:10" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:10" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:10" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:10" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:10" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:10" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:8" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" spans="1:8" ht="28.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1819,7 +1854,7 @@
         <v>46</v>
       </c>
       <c r="C59" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>86</v>
@@ -2760,7 +2795,7 @@
       </c>
     </row>
     <row r="227" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="42" t="s">
+      <c r="A227" s="43" t="s">
         <v>51</v>
       </c>
       <c r="B227" s="6" t="s">
@@ -2783,7 +2818,7 @@
       </c>
     </row>
     <row r="228" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="42"/>
+      <c r="A228" s="43"/>
       <c r="B228" s="6" t="s">
         <v>21</v>
       </c>
@@ -2804,7 +2839,7 @@
       </c>
     </row>
     <row r="229" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="42"/>
+      <c r="A229" s="43"/>
       <c r="B229" s="6" t="s">
         <v>149</v>
       </c>
@@ -2825,7 +2860,7 @@
       </c>
     </row>
     <row r="230" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="42"/>
+      <c r="A230" s="43"/>
       <c r="B230" s="6" t="s">
         <v>131</v>
       </c>
@@ -2846,7 +2881,7 @@
       </c>
     </row>
     <row r="231" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="42"/>
+      <c r="A231" s="43"/>
       <c r="B231" s="6" t="s">
         <v>5</v>
       </c>
@@ -2867,7 +2902,7 @@
       </c>
     </row>
     <row r="232" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="42"/>
+      <c r="A232" s="43"/>
       <c r="B232" s="6" t="s">
         <v>152</v>
       </c>
@@ -2888,7 +2923,7 @@
       </c>
     </row>
     <row r="233" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="42"/>
+      <c r="A233" s="43"/>
       <c r="B233" s="6" t="s">
         <v>30</v>
       </c>
@@ -2909,7 +2944,7 @@
       </c>
     </row>
     <row r="234" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="42"/>
+      <c r="A234" s="43"/>
       <c r="B234" s="6" t="s">
         <v>16</v>
       </c>
@@ -2930,7 +2965,7 @@
       </c>
     </row>
     <row r="235" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="42"/>
+      <c r="A235" s="43"/>
       <c r="B235" s="6" t="s">
         <v>6</v>
       </c>
@@ -2951,7 +2986,7 @@
       </c>
     </row>
     <row r="236" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="42"/>
+      <c r="A236" s="43"/>
       <c r="B236" s="6" t="s">
         <v>8</v>
       </c>
@@ -2972,7 +3007,7 @@
       </c>
     </row>
     <row r="237" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="42"/>
+      <c r="A237" s="43"/>
       <c r="B237" s="6" t="s">
         <v>7</v>
       </c>
@@ -2993,7 +3028,7 @@
       </c>
     </row>
     <row r="238" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="42"/>
+      <c r="A238" s="43"/>
       <c r="B238" s="6" t="s">
         <v>9</v>
       </c>
@@ -3014,7 +3049,7 @@
       </c>
     </row>
     <row r="239" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="42"/>
+      <c r="A239" s="43"/>
       <c r="B239" s="6" t="s">
         <v>11</v>
       </c>
@@ -3035,7 +3070,7 @@
       </c>
     </row>
     <row r="240" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="42"/>
+      <c r="A240" s="43"/>
       <c r="B240" s="6" t="s">
         <v>12</v>
       </c>
@@ -3056,7 +3091,7 @@
       </c>
     </row>
     <row r="241" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="42"/>
+      <c r="A241" s="43"/>
       <c r="B241" s="6" t="s">
         <v>27</v>
       </c>
@@ -3137,7 +3172,7 @@
       </c>
     </row>
     <row r="245" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="45" t="s">
+      <c r="A245" s="46" t="s">
         <v>170</v>
       </c>
       <c r="B245" s="6" t="s">
@@ -3160,7 +3195,7 @@
       </c>
     </row>
     <row r="246" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A246" s="45"/>
+      <c r="A246" s="46"/>
       <c r="B246" s="6" t="s">
         <v>158</v>
       </c>

</xml_diff>